<commit_message>
updated list of BOM
</commit_message>
<xml_diff>
--- a/Architecture/ARC BOT Major Component BOM .xlsx
+++ b/Architecture/ARC BOT Major Component BOM .xlsx
@@ -82,9 +82,6 @@
     <t>Lead Time</t>
   </si>
   <si>
-    <t>Joystick</t>
-  </si>
-  <si>
     <t>Motor (P)</t>
   </si>
   <si>
@@ -115,18 +112,6 @@
     <t>500mA</t>
   </si>
   <si>
-    <t>Audrino board</t>
-  </si>
-  <si>
-    <t>5-20 v</t>
-  </si>
-  <si>
-    <t>350mA</t>
-  </si>
-  <si>
-    <t>Audrino</t>
-  </si>
-  <si>
     <t>generic / on ebay</t>
   </si>
   <si>
@@ -151,9 +136,6 @@
     <t>total price</t>
   </si>
   <si>
-    <t>Driver board</t>
-  </si>
-  <si>
     <t>TI</t>
   </si>
   <si>
@@ -161,6 +143,24 @@
   </si>
   <si>
     <t>5v</t>
+  </si>
+  <si>
+    <t xml:space="preserve">28BYJ-48 </t>
+  </si>
+  <si>
+    <t>5 v</t>
+  </si>
+  <si>
+    <t>generic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Collision sensor limit switch module </t>
+  </si>
+  <si>
+    <t>Joystick breakout board module</t>
+  </si>
+  <si>
+    <t>Driver board module</t>
   </si>
 </sst>
 </file>
@@ -661,11 +661,12 @@
   <dimension ref="A1:M16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K24" sqref="K24"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
+    <col min="1" max="1" width="28.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.6640625" customWidth="1"/>
     <col min="3" max="3" width="8.33203125" customWidth="1"/>
     <col min="4" max="4" width="9.6640625" customWidth="1"/>
@@ -684,7 +685,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
@@ -702,7 +703,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
@@ -808,7 +809,7 @@
         <v>12</v>
       </c>
       <c r="J7" s="17" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="K7" s="17" t="s">
         <v>13</v>
@@ -833,13 +834,13 @@
     </row>
     <row r="9" spans="1:13" ht="15.75" customHeight="1">
       <c r="A9" s="10" t="s">
-        <v>20</v>
+        <v>45</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D9" s="11"/>
       <c r="E9" s="11">
@@ -847,10 +848,10 @@
         <v>0.05</v>
       </c>
       <c r="F9" s="11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G9" s="11" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="H9" s="14">
         <v>2</v>
@@ -868,19 +869,19 @@
     </row>
     <row r="10" spans="1:13" ht="15.75" customHeight="1">
       <c r="A10" s="15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="C10" s="11"/>
       <c r="D10" s="11"/>
       <c r="E10" s="11"/>
       <c r="F10" s="11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G10" s="11" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="H10" s="14">
         <v>8</v>
@@ -898,29 +899,29 @@
     </row>
     <row r="11" spans="1:13" ht="15.75" customHeight="1">
       <c r="A11" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11" s="11" t="s">
         <v>31</v>
-      </c>
-      <c r="B11" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="C11" s="11" t="s">
-        <v>33</v>
       </c>
       <c r="D11" s="11"/>
       <c r="E11" s="11"/>
       <c r="F11" s="11" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="G11" s="11"/>
       <c r="H11" s="14">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="I11" s="11">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J11" s="11">
-        <f>H11*I11</f>
-        <v>20</v>
+        <f t="shared" si="0"/>
+        <v>12</v>
       </c>
       <c r="K11" s="11"/>
       <c r="L11" s="13"/>
@@ -928,22 +929,22 @@
     </row>
     <row r="12" spans="1:13" s="11" customFormat="1" ht="15.75" customHeight="1">
       <c r="A12" s="11" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E12" s="11">
         <v>1.5</v>
       </c>
       <c r="F12" s="11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G12" s="11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H12" s="14">
         <v>4</v>
@@ -956,32 +957,32 @@
         <v>8</v>
       </c>
       <c r="K12" s="11" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="L12" s="11" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="M12" s="18"/>
     </row>
     <row r="13" spans="1:13" ht="15.75" customHeight="1">
       <c r="A13" s="15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D13" s="11"/>
       <c r="E13" s="11">
         <v>15</v>
       </c>
       <c r="F13" s="11" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="G13" s="11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H13" s="14">
         <v>15</v>
@@ -994,10 +995,10 @@
         <v>15</v>
       </c>
       <c r="K13" s="11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L13" s="13" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="M13" s="4"/>
     </row>
@@ -1013,7 +1014,7 @@
       <c r="I14" s="9"/>
       <c r="J14" s="8">
         <f>SUM(J9:J13)</f>
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="K14" s="9"/>
       <c r="L14" s="9"/>

</xml_diff>